<commit_message>
Added functionalities to all admin use classes
</commit_message>
<xml_diff>
--- a/Admins.xlsx
+++ b/Admins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming Projects\Mobile Banking App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{112471A7-A011-4073-B2CA-29A7AA34C6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E9C8DB-F4B0-4E3A-B999-4EFFABE89343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C8E62F1-5EA0-45E8-A53A-4332C4C81AF0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -36,22 +36,19 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Kavish</t>
-  </si>
-  <si>
-    <t>kavish</t>
-  </si>
-  <si>
-    <t>kavish1234</t>
-  </si>
-  <si>
-    <t>Preet</t>
-  </si>
-  <si>
-    <t>preet</t>
-  </si>
-  <si>
-    <t>preet1234</t>
+    <t>Sample1</t>
+  </si>
+  <si>
+    <t>sample1</t>
+  </si>
+  <si>
+    <t>sample1234</t>
+  </si>
+  <si>
+    <t>Sample2</t>
+  </si>
+  <si>
+    <t>sample2</t>
   </si>
 </sst>
 </file>
@@ -406,7 +403,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>